<commit_message>
the commit has been made
</commit_message>
<xml_diff>
--- a/src/test/java/resources/ulkeler.xlsx
+++ b/src/test/java/resources/ulkeler.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="575">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1740,12 +1740,19 @@
   </si>
   <si>
     <t>Zimbabve</t>
+  </si>
+  <si>
+    <t>NUFUS</t>
+  </si>
+  <si>
+    <t>5000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2166,7 +2173,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -2174,7 +2181,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="25.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2190,6 +2197,9 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -2245,6 +2255,9 @@
       </c>
       <c r="D5" s="7" t="s">
         <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>